<commit_message>
:recycle: remake when blogging
</commit_message>
<xml_diff>
--- a/Statistics/Instruction.xlsx
+++ b/Statistics/Instruction.xlsx
@@ -10,14 +10,15 @@
     <sheet name="instructionCount" sheetId="1" r:id="rId1"/>
     <sheet name="instructionType" sheetId="2" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
-    <sheet name="Chart" sheetId="4" r:id="rId4"/>
+    <sheet name="StatisticsType" sheetId="4" r:id="rId4"/>
+    <sheet name="Chart" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="173">
   <si>
     <t>Instruction</t>
   </si>
@@ -533,6 +534,9 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Numbers</t>
   </si>
 </sst>
 </file>
@@ -5427,6 +5431,74 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2">
+        <v>93</v>
+      </c>
+      <c r="C2">
+        <v>38514</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>12981</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>8016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>1703</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>